<commit_message>
exporting most cleaned cohort data
</commit_message>
<xml_diff>
--- a/cohorts2/ref/cohorts1-prev/raw/NF1 Glioma Pathology Reports.xlsx
+++ b/cohorts2/ref/cohorts1-prev/raw/NF1 Glioma Pathology Reports.xlsx
@@ -910,8 +910,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A52921E31622BA47A5BEE7A2CE318F26" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="72c5dd4de6ee2a9f5337ff02160f23b1">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="98fb7176-381e-4eb6-825b-93e64c92b6ea" xmlns:ns3="fe56dbcb-f404-42a8-8006-471f9c1a2fc9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c7858ab809dd018e06c72c2e5abe05b4" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A52921E31622BA47A5BEE7A2CE318F26" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bbbe4ce2f8fe09d1c797aa555d1ed32a">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="98fb7176-381e-4eb6-825b-93e64c92b6ea" xmlns:ns3="fe56dbcb-f404-42a8-8006-471f9c1a2fc9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1e562a0e15c5e5c6d0c89a0f84659810" ns2:_="" ns3:_="">
     <xsd:import namespace="98fb7176-381e-4eb6-825b-93e64c92b6ea"/>
     <xsd:import namespace="fe56dbcb-f404-42a8-8006-471f9c1a2fc9"/>
     <xsd:element name="properties">
@@ -929,6 +929,8 @@
                 <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -981,6 +983,16 @@
     <xsd:element name="MediaServiceLocation" ma:index="17" nillable="true" ma:displayName="Location" ma:indexed="true" ma:internalName="MediaServiceLocation" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="18" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:description="" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="19" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -1107,10 +1119,25 @@
 </FormTemplates>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="fe56dbcb-f404-42a8-8006-471f9c1a2fc9" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="98fb7176-381e-4eb6-825b-93e64c92b6ea">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BEADE5F-2DD0-48A0-81F3-6730D2589680}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{35D05E1A-BD5A-47F0-B926-EA9A180619DF}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9728F90D-35F1-4B9E-AA50-989AC1A2C3A5}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11C02007-9C9B-471D-86D8-6442365E17B9}"/>
 </file>
</xml_diff>